<commit_message>
chore: snapshot working state before branch consolidation
- Updated Batchdata_Template.xlsx
- Updated v300Dialer_template.xlsx
- Added BD_PREFIX_MIGRATION_COMPLETE.md
- Added Batchdata/BD_PREFIX_MIGRATION.md
- Added branching-strategy-conservative.md

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/v300Dialer_template.xlsx
+++ b/v300Dialer_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED2C9F8-46F9-F243-B060-9621AC0BD4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E945BAE4-6E6E-0E46-949B-9D764C241DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="0" windowWidth="17480" windowHeight="22400" activeTab="1" xr2:uid="{18482702-A69E-6041-904C-3409D379D533}"/>
+    <workbookView xWindow="18360" yWindow="0" windowWidth="17480" windowHeight="22400" activeTab="2" xr2:uid="{18482702-A69E-6041-904C-3409D379D533}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="664">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -1719,12 +1720,336 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>LAST DATE I CALLED</t>
+  </si>
+  <si>
+    <t>LAST DATE THEY PICKED UP</t>
+  </si>
+  <si>
+    <t>for these, can do a click display where colors of the nodes/icons tell you if 1) you called, no answer, voicemail 2)  you called, no answer, no voicemail, proceed horizontally where upon click</t>
+  </si>
+  <si>
+    <t>BD_RECORD_ID</t>
+  </si>
+  <si>
+    <t>BD_SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t>BD_ENTITY_NAME</t>
+  </si>
+  <si>
+    <t>BD_SOURCE_ENTITY_ID</t>
+  </si>
+  <si>
+    <t>BD_TITLE_ROLE</t>
+  </si>
+  <si>
+    <t>BD_TARGET_FIRST_NAME</t>
+  </si>
+  <si>
+    <t>BD_TARGET_LAST_NAME</t>
+  </si>
+  <si>
+    <t>BD_OWNER_NAME_FULL</t>
+  </si>
+  <si>
+    <t>BD_ADDRESS</t>
+  </si>
+  <si>
+    <t>BD_ADDRESS_2</t>
+  </si>
+  <si>
+    <t>BD_STATE</t>
+  </si>
+  <si>
+    <t>BD_MAILING_LINE1</t>
+  </si>
+  <si>
+    <t>BD_MAILING_CITY</t>
+  </si>
+  <si>
+    <t>BD_MAILING_STATE</t>
+  </si>
+  <si>
+    <t>BD_MAILING_ZIP</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_TYPE</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_CARRIER</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_DNC</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_TCPA</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_1</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_1_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_2</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_2_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_3</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_3_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_4</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_4_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_5</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_5_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_6</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_6_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_7</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_7_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_8</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_8_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_9</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_9_TESTED</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_10</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_10_TESTED</t>
+  </si>
+  <si>
+    <t>BD_API_STATUS</t>
+  </si>
+  <si>
+    <t>BD_API_RESPONSE_TIME</t>
+  </si>
+  <si>
+    <t>BD_PERSONS_FOUND</t>
+  </si>
+  <si>
+    <t>BD_PHONES_FOUND</t>
+  </si>
+  <si>
+    <t>BD_EMAILS_FOUND</t>
+  </si>
+  <si>
+    <t>BD_PIPELINE_VERSION</t>
+  </si>
+  <si>
+    <t>BD_PIPELINE_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>BD_STAGES_APPLIED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1798,8 +2123,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1854,8 +2185,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAF2D0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1889,12 +2226,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1984,12 +2334,52 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2011,6 +2401,429 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B655DDB5-2D84-624D-9FEF-848E85EF2906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="2438400"/>
+          <a:ext cx="15798800" cy="8750300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>1x ADDRESS per RECORD</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>(unlike Ecorp Where it was one name and multiple addresses and contact information, and names per record.)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>How are Addresses linked</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> with people linked with phone numbers. No consistancy.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>ADDRESS &amp; INDIV CENTERED "Hi, I'm hoping to get in contact with INDIV about the ADDRESS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Manager/Member - 5 Phone Numbers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Member - 5 Phone Numbers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>ACTIONS:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> We are renaming fields &amp; this should update all logic and mention of the previously titled field as to not disrupt funcitonality. This means update </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>Ecorp/Ecorp_template_fields_desc.md  and other. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>I have updated the fields naming in Ecorp_Template.xlsx... </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>this could Be as simple as changing the red, the ones that are going into batch data for naming just conventions, i.e., change Comments to ECORP_COMMENTS. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Also rename County to ECORP_COUNTY</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+          </a:br>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2) ANALYSIS on overlap of phone numbers &amp; strategy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> as each address gives up to 10 numbers. &amp; we need to filter out the DNC.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Good thinking, yeah lets map it, No need to move columns at all:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> 'address_line1' will be ‘BD_ADDRESS’ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>'city' to ‘BD_CITY’</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> 'state' to ‘BD_STATE’ - </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> - zip' to ‘BD_ZIP’ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> 'record_id' to ‘BD_RECORD_ID’ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>QUESTIONS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> ABOUT CURRENT ECORP_COMPLETE:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>1) Is Domicile State the state associated with an individuals ADDRESS being scraped from site or just where the entity is based out of (no individual relationship)? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>NO INDIV RELATIONSHIP</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>2) Same thing for Couty</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3) Where is the Ecorp_Template</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> defined fields for population logic? If none, create .md </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>NOW at Ecorp/Ecorp_template_fields_desc.md </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>4) Is Batchdata Template going to serve as the input and output? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>YES</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0"/>
+            <a:t>5) Is there any logic to where Owner_Ownership &amp; Search Name columns can ever be different populated values? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>YES, for INDIVIDUALS Search Name is always blank</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1"/>
+            <a:t>CODEBASE OVERALL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t> QUESTION:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>1) Should there be no repeat naming i.e. Analysis has FULL_ADDRESS and so does MCAO_Complete and so will Batchdata -- All this in v300 Dialer seems wrong no?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2330,11 +3143,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA547D1D-55E4-9142-B57A-C035D375D836}">
-  <dimension ref="A1:JR37"/>
+  <dimension ref="A1:JR36"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D19"/>
-    </sheetView>
+    <sheetView zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3965,366 +4776,104 @@
         <v>342</v>
       </c>
     </row>
-    <row r="36" spans="2:126" x14ac:dyDescent="0.2">
-      <c r="S36" t="s">
-        <v>488</v>
-      </c>
-      <c r="T36" t="s">
-        <v>489</v>
-      </c>
-      <c r="U36" t="s">
-        <v>490</v>
-      </c>
-      <c r="V36" t="s">
-        <v>491</v>
-      </c>
-      <c r="W36" t="s">
-        <v>492</v>
-      </c>
+    <row r="36" spans="2:93" x14ac:dyDescent="0.2">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
       <c r="X36"/>
       <c r="Y36"/>
-      <c r="Z36" t="s">
-        <v>493</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>494</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>495</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>496</v>
-      </c>
-      <c r="AD36" t="s">
-        <v>497</v>
-      </c>
-      <c r="AE36">
-        <v>85282</v>
-      </c>
-      <c r="AF36" t="s">
-        <v>498</v>
-      </c>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
       <c r="AG36"/>
       <c r="AH36"/>
       <c r="AI36"/>
       <c r="AJ36"/>
       <c r="AK36"/>
-      <c r="AL36" t="s">
-        <v>499</v>
-      </c>
-      <c r="AM36" t="s">
-        <v>500</v>
-      </c>
-      <c r="AN36" t="s">
-        <v>501</v>
-      </c>
-      <c r="AO36" t="s">
-        <v>502</v>
-      </c>
-      <c r="AP36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ36" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR36">
-        <v>100</v>
-      </c>
-      <c r="AS36" t="s">
-        <v>503</v>
-      </c>
-      <c r="AT36" t="s">
-        <v>504</v>
-      </c>
-      <c r="AU36" t="s">
-        <v>505</v>
-      </c>
-      <c r="AV36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW36" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX36">
-        <v>95</v>
-      </c>
-      <c r="AY36" t="s">
-        <v>506</v>
-      </c>
-      <c r="AZ36" t="s">
-        <v>504</v>
-      </c>
-      <c r="BA36" t="s">
-        <v>507</v>
-      </c>
-      <c r="BB36" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD36">
-        <v>90</v>
-      </c>
-      <c r="BE36" t="s">
-        <v>508</v>
-      </c>
-      <c r="BF36" t="s">
-        <v>504</v>
-      </c>
-      <c r="BG36" t="s">
-        <v>507</v>
-      </c>
-      <c r="BH36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BI36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ36">
-        <v>85</v>
-      </c>
-      <c r="BK36" t="s">
-        <v>509</v>
-      </c>
-      <c r="BL36" t="s">
-        <v>504</v>
-      </c>
-      <c r="BM36" t="s">
-        <v>510</v>
-      </c>
-      <c r="BN36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BO36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BP36">
-        <v>80</v>
-      </c>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+      <c r="BE36"/>
+      <c r="BF36"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+      <c r="BI36"/>
+      <c r="BJ36"/>
+      <c r="BK36"/>
+      <c r="BL36"/>
+      <c r="BM36"/>
+      <c r="BN36"/>
+      <c r="BO36"/>
+      <c r="BP36"/>
       <c r="BQ36"/>
       <c r="BR36"/>
       <c r="BS36"/>
-      <c r="BT36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BU36" t="b">
-        <v>0</v>
-      </c>
-      <c r="BV36">
-        <v>0</v>
-      </c>
+      <c r="BT36"/>
+      <c r="BU36"/>
+      <c r="BV36"/>
       <c r="BW36"/>
       <c r="BX36"/>
       <c r="BY36"/>
-      <c r="BZ36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CA36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CB36">
-        <v>0</v>
-      </c>
+      <c r="BZ36"/>
+      <c r="CA36"/>
+      <c r="CB36"/>
       <c r="CC36"/>
       <c r="CD36"/>
       <c r="CE36"/>
-      <c r="CF36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CG36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CH36">
-        <v>0</v>
-      </c>
+      <c r="CF36"/>
+      <c r="CG36"/>
+      <c r="CH36"/>
       <c r="CI36"/>
       <c r="CJ36"/>
       <c r="CK36"/>
-      <c r="CL36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CM36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CN36">
-        <v>0</v>
-      </c>
+      <c r="CL36"/>
+      <c r="CM36"/>
+      <c r="CN36"/>
       <c r="CO36"/>
-      <c r="CP36"/>
-      <c r="CQ36"/>
-      <c r="CR36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CS36" t="b">
-        <v>0</v>
-      </c>
-      <c r="CT36">
-        <v>0</v>
-      </c>
-      <c r="CU36"/>
-      <c r="CV36" t="b">
-        <v>1</v>
-      </c>
-      <c r="CW36"/>
-      <c r="CX36" t="b">
-        <v>1</v>
-      </c>
-      <c r="CY36"/>
-      <c r="CZ36" t="b">
-        <v>1</v>
-      </c>
-      <c r="DA36"/>
-      <c r="DB36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DC36"/>
-      <c r="DD36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DE36"/>
-      <c r="DF36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DG36"/>
-      <c r="DH36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DI36"/>
-      <c r="DJ36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DK36"/>
-      <c r="DL36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DM36"/>
-      <c r="DN36" t="b">
-        <v>0</v>
-      </c>
-      <c r="DO36" t="s">
-        <v>511</v>
-      </c>
-      <c r="DP36" t="s">
-        <v>512</v>
-      </c>
-      <c r="DQ36">
-        <v>1</v>
-      </c>
-      <c r="DR36">
-        <v>5</v>
-      </c>
-      <c r="DS36">
-        <v>3</v>
-      </c>
-      <c r="DT36" t="s">
-        <v>513</v>
-      </c>
-      <c r="DU36" t="s">
-        <v>514</v>
-      </c>
-      <c r="DV36" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="37" spans="2:126" x14ac:dyDescent="0.2">
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-      <c r="AR37"/>
-      <c r="AS37"/>
-      <c r="AT37"/>
-      <c r="AU37"/>
-      <c r="AV37"/>
-      <c r="AW37"/>
-      <c r="AX37"/>
-      <c r="AY37"/>
-      <c r="AZ37"/>
-      <c r="BA37"/>
-      <c r="BB37"/>
-      <c r="BC37"/>
-      <c r="BD37"/>
-      <c r="BE37"/>
-      <c r="BF37"/>
-      <c r="BG37"/>
-      <c r="BH37"/>
-      <c r="BI37"/>
-      <c r="BJ37"/>
-      <c r="BK37"/>
-      <c r="BL37"/>
-      <c r="BM37"/>
-      <c r="BN37"/>
-      <c r="BO37"/>
-      <c r="BP37"/>
-      <c r="BQ37"/>
-      <c r="BR37"/>
-      <c r="BS37"/>
-      <c r="BT37"/>
-      <c r="BU37"/>
-      <c r="BV37"/>
-      <c r="BW37"/>
-      <c r="BX37"/>
-      <c r="BY37"/>
-      <c r="BZ37"/>
-      <c r="CA37"/>
-      <c r="CB37"/>
-      <c r="CC37"/>
-      <c r="CD37"/>
-      <c r="CE37"/>
-      <c r="CF37"/>
-      <c r="CG37"/>
-      <c r="CH37"/>
-      <c r="CI37"/>
-      <c r="CJ37"/>
-      <c r="CK37"/>
-      <c r="CL37"/>
-      <c r="CM37"/>
-      <c r="CN37"/>
-      <c r="CO37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4335,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CC8DD6-553E-B042-A242-6B3867F459A2}">
   <dimension ref="A1:FA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6366,6 +6915,236 @@
         <v>467</v>
       </c>
     </row>
+    <row r="9" spans="1:157" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>488</v>
+      </c>
+      <c r="T9" t="s">
+        <v>489</v>
+      </c>
+      <c r="U9" t="s">
+        <v>490</v>
+      </c>
+      <c r="V9" t="s">
+        <v>491</v>
+      </c>
+      <c r="W9" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>493</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>494</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>495</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>496</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE9">
+        <v>85282</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>498</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>499</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>500</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>501</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>502</v>
+      </c>
+      <c r="AP9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>100</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>503</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>504</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>505</v>
+      </c>
+      <c r="AV9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>95</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>506</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>504</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>507</v>
+      </c>
+      <c r="BB9" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>90</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>508</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>504</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>507</v>
+      </c>
+      <c r="BH9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BJ9">
+        <v>85</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>509</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>504</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>510</v>
+      </c>
+      <c r="BN9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BO9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BP9">
+        <v>80</v>
+      </c>
+      <c r="BT9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BU9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BV9">
+        <v>0</v>
+      </c>
+      <c r="BZ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CA9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CB9">
+        <v>0</v>
+      </c>
+      <c r="CF9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CG9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH9">
+        <v>0</v>
+      </c>
+      <c r="CL9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CM9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CN9">
+        <v>0</v>
+      </c>
+      <c r="CR9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CS9" t="b">
+        <v>0</v>
+      </c>
+      <c r="CT9">
+        <v>0</v>
+      </c>
+      <c r="CV9" t="b">
+        <v>1</v>
+      </c>
+      <c r="CX9" t="b">
+        <v>1</v>
+      </c>
+      <c r="CZ9" t="b">
+        <v>1</v>
+      </c>
+      <c r="DB9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DD9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DF9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DH9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DJ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DL9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DN9" t="b">
+        <v>0</v>
+      </c>
+      <c r="DO9" t="s">
+        <v>511</v>
+      </c>
+      <c r="DP9" t="s">
+        <v>512</v>
+      </c>
+      <c r="DQ9">
+        <v>1</v>
+      </c>
+      <c r="DR9">
+        <v>5</v>
+      </c>
+      <c r="DS9">
+        <v>3</v>
+      </c>
+      <c r="DT9" t="s">
+        <v>513</v>
+      </c>
+      <c r="DU9" t="s">
+        <v>514</v>
+      </c>
+      <c r="DV9" t="s">
+        <v>515</v>
+      </c>
+    </row>
     <row r="14" spans="1:157" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
@@ -6499,25 +7278,25 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="25" t="s">
         <v>528</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="25" t="s">
         <v>555</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="25" t="s">
         <v>529</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="25" t="s">
         <v>555</v>
       </c>
       <c r="D27" s="1"/>
@@ -6542,4 +7321,1244 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC910AD2-6A54-CE44-98F5-4DD48CB453A6}">
+  <dimension ref="A1:OK4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="JM1" workbookViewId="0">
+      <selection activeCell="IU1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:401" ht="80" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG1" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH1" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI1" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL1" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM1" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN1" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO1" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP1" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ1" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="AR1" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS1" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT1" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU1" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV1" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW1" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX1" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="AY1" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ1" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA1" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB1" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="BC1" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD1" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE1" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="BF1" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG1" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH1" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="BI1" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="BJ1" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK1" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="BL1" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="BM1" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="BN1" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="BO1" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="BP1" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="BQ1" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="BR1" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="BS1" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT1" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU1" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW1" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="BX1" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="BY1" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BZ1" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="CA1" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="CB1" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="CC1" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="CD1" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="CE1" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="CF1" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="CG1" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="CH1" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="CI1" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="CJ1" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="CK1" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="CL1" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="CM1" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN1" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="CO1" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="CP1" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="CQ1" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="CR1" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="CS1" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="CT1" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="CU1" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="CV1" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="CW1" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="CX1" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="CY1" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="CZ1" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="DA1" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="DB1" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="DC1" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="DD1" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="DE1" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="DF1" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="DG1" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="DH1" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="DI1" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="DJ1" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="DK1" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="DL1" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="DM1" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="DN1" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="DO1" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="DP1" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="DQ1" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="DR1" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="DS1" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="DT1" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="DU1" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="DV1" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="DW1" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="DX1" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="DY1" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="DZ1" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="EA1" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="EB1" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="EC1" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="ED1" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="EE1" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="EF1" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="EG1" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="EH1" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="EI1" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="EJ1" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="EK1" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="EL1" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="EM1" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="EN1" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="EO1" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="EP1" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="EQ1" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="ER1" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="ES1" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="ET1" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="EU1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="EV1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="EW1" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="EX1" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="EY1" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="EZ1" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="FA1" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="FB1" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="FC1" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="FD1" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="FE1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="FF1" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="FG1" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="FH1" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="FI1" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="FJ1" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="FK1" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="FL1" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="FM1" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="FN1" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="FO1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="FP1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="FQ1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="FR1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="FS1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="FT1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="FU1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="FV1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="FW1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="FX1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="FY1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="FZ1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="GA1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="GB1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="GC1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="GD1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="GE1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="GF1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="GH1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="GI1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="GJ1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="GK1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="GL1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="GM1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="GN1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="GO1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="GP1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="GQ1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="GR1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="GS1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="GT1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="GU1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="GV1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="GW1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="GX1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="GY1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="GZ1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="HA1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="HB1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="HC1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="HD1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="HE1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="HF1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="HG1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="HH1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="HI1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="HJ1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="HK1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="HL1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="HM1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="HN1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="HO1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="HP1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="HQ1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="HR1" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="HS1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="HT1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="HU1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="HV1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="HW1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="HX1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="HY1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="HZ1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="IA1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="IB1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="IC1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="ID1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="IE1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="IF1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="IG1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="IH1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="II1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="IJ1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="IK1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="IL1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="IM1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="IN1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="IO1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="IP1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="IQ1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="IR1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="IS1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="IT1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="IU1" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="IV1" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="IW1" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="IX1" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="IY1" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="IZ1" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="JA1" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="JB1" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="JC1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="JD1" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="JE1" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="JF1" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="JG1" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="JH1" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="JI1" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="JJ1" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="JK1" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="JL1" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="JM1" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="JN1" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="JO1" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="JP1" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="JQ1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="JR1" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="JS1" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="JT1" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="JU1" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="JV1" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="JW1" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="JX1" s="30" t="s">
+        <v>532</v>
+      </c>
+      <c r="JY1" s="30" t="s">
+        <v>533</v>
+      </c>
+      <c r="JZ1" s="30" t="s">
+        <v>534</v>
+      </c>
+      <c r="KA1" s="30" t="s">
+        <v>535</v>
+      </c>
+      <c r="KB1" s="30" t="s">
+        <v>536</v>
+      </c>
+      <c r="KC1" s="30" t="s">
+        <v>537</v>
+      </c>
+      <c r="KD1" s="30" t="s">
+        <v>538</v>
+      </c>
+      <c r="KE1" s="30" t="s">
+        <v>539</v>
+      </c>
+      <c r="KF1" s="30" t="s">
+        <v>540</v>
+      </c>
+      <c r="KG1" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="KH1" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="KI1" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="KJ1" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="KK1" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="KL1" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="KM1" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="KN1" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="KO1" s="28" t="s">
+        <v>568</v>
+      </c>
+      <c r="KP1" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="KQ1" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="KR1" s="28" t="s">
+        <v>548</v>
+      </c>
+      <c r="KS1" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="KT1" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="KU1" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="KV1" s="28" t="s">
+        <v>551</v>
+      </c>
+      <c r="KW1" s="28" t="s">
+        <v>572</v>
+      </c>
+      <c r="KX1" s="28" t="s">
+        <v>573</v>
+      </c>
+      <c r="KY1" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="KZ1" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="LA1" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="LB1" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="LC1" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="LD1" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="LE1" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="LF1" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="LG1" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="LH1" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="LI1" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="LJ1" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="LK1" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="LL1" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="LM1" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="LN1" s="28" t="s">
+        <v>588</v>
+      </c>
+      <c r="LO1" s="28" t="s">
+        <v>589</v>
+      </c>
+      <c r="LP1" s="28" t="s">
+        <v>590</v>
+      </c>
+      <c r="LQ1" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="LR1" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="LS1" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="LT1" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="LU1" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="LV1" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="LW1" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="LX1" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="LY1" s="28" t="s">
+        <v>599</v>
+      </c>
+      <c r="LZ1" s="28" t="s">
+        <v>600</v>
+      </c>
+      <c r="MA1" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="MB1" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="MC1" s="28" t="s">
+        <v>603</v>
+      </c>
+      <c r="MD1" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="ME1" s="28" t="s">
+        <v>605</v>
+      </c>
+      <c r="MF1" s="28" t="s">
+        <v>606</v>
+      </c>
+      <c r="MG1" s="28" t="s">
+        <v>607</v>
+      </c>
+      <c r="MH1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="MI1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="MJ1" s="28" t="s">
+        <v>610</v>
+      </c>
+      <c r="MK1" s="28" t="s">
+        <v>611</v>
+      </c>
+      <c r="ML1" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="MM1" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="MN1" s="28" t="s">
+        <v>614</v>
+      </c>
+      <c r="MO1" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="MP1" s="28" t="s">
+        <v>616</v>
+      </c>
+      <c r="MQ1" s="28" t="s">
+        <v>617</v>
+      </c>
+      <c r="MR1" s="28" t="s">
+        <v>618</v>
+      </c>
+      <c r="MS1" s="28" t="s">
+        <v>619</v>
+      </c>
+      <c r="MT1" s="28" t="s">
+        <v>620</v>
+      </c>
+      <c r="MU1" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="MV1" s="28" t="s">
+        <v>622</v>
+      </c>
+      <c r="MW1" s="28" t="s">
+        <v>623</v>
+      </c>
+      <c r="MX1" s="28" t="s">
+        <v>624</v>
+      </c>
+      <c r="MY1" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="MZ1" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="NA1" s="28" t="s">
+        <v>627</v>
+      </c>
+      <c r="NB1" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="NC1" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="ND1" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="NE1" s="28" t="s">
+        <v>631</v>
+      </c>
+      <c r="NF1" s="28" t="s">
+        <v>632</v>
+      </c>
+      <c r="NG1" s="28" t="s">
+        <v>633</v>
+      </c>
+      <c r="NH1" s="28" t="s">
+        <v>634</v>
+      </c>
+      <c r="NI1" s="28" t="s">
+        <v>635</v>
+      </c>
+      <c r="NJ1" s="28" t="s">
+        <v>636</v>
+      </c>
+      <c r="NK1" s="28" t="s">
+        <v>637</v>
+      </c>
+      <c r="NL1" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="NM1" s="28" t="s">
+        <v>639</v>
+      </c>
+      <c r="NN1" s="28" t="s">
+        <v>640</v>
+      </c>
+      <c r="NO1" s="28" t="s">
+        <v>641</v>
+      </c>
+      <c r="NP1" s="28" t="s">
+        <v>642</v>
+      </c>
+      <c r="NQ1" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="NR1" s="28" t="s">
+        <v>644</v>
+      </c>
+      <c r="NS1" s="28" t="s">
+        <v>645</v>
+      </c>
+      <c r="NT1" s="28" t="s">
+        <v>646</v>
+      </c>
+      <c r="NU1" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="NV1" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="NW1" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="NX1" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="NY1" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="NZ1" s="28" t="s">
+        <v>652</v>
+      </c>
+      <c r="OA1" s="28" t="s">
+        <v>653</v>
+      </c>
+      <c r="OB1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="OC1" s="28" t="s">
+        <v>655</v>
+      </c>
+      <c r="OD1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="OE1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="OF1" s="28" t="s">
+        <v>658</v>
+      </c>
+      <c r="OG1" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="OH1" s="28" t="s">
+        <v>660</v>
+      </c>
+      <c r="OI1" s="28" t="s">
+        <v>661</v>
+      </c>
+      <c r="OJ1" s="28" t="s">
+        <v>662</v>
+      </c>
+      <c r="OK1" s="28" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:401" x14ac:dyDescent="0.2">
+      <c r="C3" s="33" t="s">
+        <v>558</v>
+      </c>
+      <c r="D3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:401" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H1:N1">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:G1">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
preserve: Copy 3 AI refactor changes (deletions deferred)
Preserved changes from Copy 3 AI refactor session:

Modified Batchdata source files:
- batchdata_sync.py
- io.py
- normalize.py
- run.py
- transform.py

Modified ETL bridge:
- src/adhs_etl/batchdata_bridge.py

Updated documentation:
- Batchdata/PIPELINE_INTEGRATION_GUIDE.md
- Batchdata/README.md

Updated templates:
- Batchdata_Template.xlsx
- v300Dialer_template.xlsx

NOTE: Copy 3 also deleted template_config.xlsx and
batchdata_local_input.xlsx, but these deletions were NOT
applied because both files have active code references
(13 and 25 references respectively).

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/v300Dialer_template.xlsx
+++ b/v300Dialer_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E945BAE4-6E6E-0E46-949B-9D764C241DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA421E7-ED6A-3542-9B93-A9AD6AEBB181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18360" yWindow="0" windowWidth="17480" windowHeight="22400" activeTab="2" xr2:uid="{18482702-A69E-6041-904C-3409D379D533}"/>
   </bookViews>
@@ -2349,17 +2349,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4873,7 +4863,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7327,8 +7317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC910AD2-6A54-CE44-98F5-4DD48CB453A6}">
   <dimension ref="A1:OK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JM1" workbookViewId="0">
-      <selection activeCell="IU1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="JC1" workbookViewId="0">
+      <selection activeCell="JK9" sqref="JK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8550,13 +8540,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:N1">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:G1">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>